<commit_message>
metadados OK, falta  para saida e vagas, vagas não roda, add dataArquivo a planilha, correção logs
</commit_message>
<xml_diff>
--- a/portal_phpcsv/uploads/AcessoPortal.xlsx
+++ b/portal_phpcsv/uploads/AcessoPortal.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>Código</t>
   </si>
@@ -33,6 +33,12 @@
   </si>
   <si>
     <t>Fatec</t>
+  </si>
+  <si>
+    <t>Data Arquivo Ori</t>
+  </si>
+  <si>
+    <t>2024-11-28 09:45:01</t>
   </si>
 </sst>
 </file>
@@ -377,7 +383,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -388,7 +394,7 @@
     <col min="5" max="5" width="17" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" customHeight="1" ht="14.25">
+    <row r="1" spans="1:6" customHeight="1" ht="14.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -404,8 +410,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" customHeight="1" ht="14.25">
       <c r="A2">
         <v>16</v>
       </c>
@@ -421,8 +430,11 @@
       <c r="E2">
         <v>239</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" customHeight="1" ht="14.25">
       <c r="A3">
         <v>17</v>
       </c>
@@ -438,8 +450,11 @@
       <c r="E3">
         <v>238</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" customHeight="1" ht="14.25">
       <c r="A4">
         <v>18</v>
       </c>
@@ -455,8 +470,11 @@
       <c r="E4">
         <v>412</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" customHeight="1" ht="14.25">
       <c r="A5">
         <v>19</v>
       </c>
@@ -472,8 +490,11 @@
       <c r="E5">
         <v>222</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" customHeight="1" ht="14.25">
       <c r="A6">
         <v>20</v>
       </c>
@@ -489,8 +510,11 @@
       <c r="E6">
         <v>225</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" customHeight="1" ht="14.25">
       <c r="A7">
         <v>21</v>
       </c>
@@ -506,8 +530,11 @@
       <c r="E7">
         <v>173</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" customHeight="1" ht="14.25">
       <c r="A8">
         <v>22</v>
       </c>
@@ -523,8 +550,11 @@
       <c r="E8">
         <v>187</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" customHeight="1" ht="14.25">
       <c r="A9">
         <v>23</v>
       </c>
@@ -540,8 +570,11 @@
       <c r="E9">
         <v>243</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" customHeight="1" ht="14.25">
       <c r="A10">
         <v>24</v>
       </c>
@@ -557,8 +590,11 @@
       <c r="E10">
         <v>179</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" customHeight="1" ht="14.25">
       <c r="A11">
         <v>25</v>
       </c>
@@ -574,8 +610,11 @@
       <c r="E11">
         <v>146</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" customHeight="1" ht="14.25">
       <c r="A12">
         <v>26</v>
       </c>
@@ -591,8 +630,11 @@
       <c r="E12">
         <v>149</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" customHeight="1" ht="14.25">
       <c r="A13">
         <v>27</v>
       </c>
@@ -608,8 +650,11 @@
       <c r="E13">
         <v>156</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" customHeight="1" ht="14.25">
       <c r="A14">
         <v>28</v>
       </c>
@@ -625,8 +670,11 @@
       <c r="E14">
         <v>220</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" customHeight="1" ht="14.25">
       <c r="A15">
         <v>29</v>
       </c>
@@ -642,8 +690,11 @@
       <c r="E15">
         <v>203</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" customHeight="1" ht="14.25">
       <c r="A16">
         <v>30</v>
       </c>
@@ -659,8 +710,11 @@
       <c r="E16">
         <v>198</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" customHeight="1" ht="14.25">
       <c r="A17">
         <v>31</v>
       </c>
@@ -676,8 +730,11 @@
       <c r="E17">
         <v>181</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" customHeight="1" ht="14.25">
       <c r="A18">
         <v>32</v>
       </c>
@@ -693,8 +750,11 @@
       <c r="E18">
         <v>496</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" customHeight="1" ht="14.25">
       <c r="A19">
         <v>33</v>
       </c>
@@ -710,8 +770,11 @@
       <c r="E19">
         <v>292</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" customHeight="1" ht="14.25">
       <c r="A20">
         <v>34</v>
       </c>
@@ -727,8 +790,11 @@
       <c r="E20">
         <v>176</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" customHeight="1" ht="14.25">
       <c r="A21">
         <v>35</v>
       </c>
@@ -744,8 +810,11 @@
       <c r="E21">
         <v>252</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" customHeight="1" ht="14.25">
       <c r="A22">
         <v>36</v>
       </c>
@@ -761,8 +830,11 @@
       <c r="E22">
         <v>231</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" customHeight="1" ht="14.25">
       <c r="A23">
         <v>37</v>
       </c>
@@ -778,8 +850,11 @@
       <c r="E23">
         <v>222</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" customHeight="1" ht="14.25">
       <c r="A24">
         <v>38</v>
       </c>
@@ -795,8 +870,11 @@
       <c r="E24">
         <v>181</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" customHeight="1" ht="14.25">
       <c r="A25">
         <v>39</v>
       </c>
@@ -812,8 +890,11 @@
       <c r="E25">
         <v>142</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" customHeight="1" ht="14.25">
       <c r="A26">
         <v>40</v>
       </c>
@@ -829,8 +910,11 @@
       <c r="E26">
         <v>224</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" customHeight="1" ht="14.25">
       <c r="A27">
         <v>41</v>
       </c>
@@ -846,8 +930,11 @@
       <c r="E27">
         <v>262</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" customHeight="1" ht="14.25">
       <c r="A28">
         <v>42</v>
       </c>
@@ -863,8 +950,11 @@
       <c r="E28">
         <v>299</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" customHeight="1" ht="14.25">
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" customHeight="1" ht="14.25">
       <c r="A29">
         <v>43</v>
       </c>
@@ -879,6 +969,9 @@
       </c>
       <c r="E29">
         <v>156</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
metadados OK e dataArquivoOriginal Ok nas 3 planilhas
</commit_message>
<xml_diff>
--- a/portal_phpcsv/uploads/AcessoPortal.xlsx
+++ b/portal_phpcsv/uploads/AcessoPortal.xlsx
@@ -35,10 +35,10 @@
     <t>Fatec</t>
   </si>
   <si>
-    <t>Data Arquivo Ori</t>
+    <t>Data Arquivo Original</t>
   </si>
   <si>
-    <t>2024-11-28 15:08:16</t>
+    <t>2024-09-03 19:09:14</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Refazer Upload, Acesso OK, problemas perda dados
</commit_message>
<xml_diff>
--- a/portal_phpcsv/uploads/AcessoPortal.xlsx
+++ b/portal_phpcsv/uploads/AcessoPortal.xlsx
@@ -35,10 +35,10 @@
     <t>Fatec</t>
   </si>
   <si>
-    <t>Data Arquivo Original</t>
+    <t>Data Arquivo Ori</t>
   </si>
   <si>
-    <t>2024-09-03 19:09:14</t>
+    <t>2024-09-03 16:09:14</t>
   </si>
 </sst>
 </file>

</xml_diff>